<commit_message>
seems to scrape properly and can now output csvs as it goes to prevent an error ruining it all. also takes in an output directory. about to test a high number of rows
</commit_message>
<xml_diff>
--- a/py_files/workfile_small_.xlsx
+++ b/py_files/workfile_small_.xlsx
@@ -1628,7 +1628,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Scraped_</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Scraped_</t>
+          <t>Scraped</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Scraped_</t>
+          <t>Scraped</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Scraped_</t>
+          <t>Scraped</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Scraped_</t>
+          <t>Scraped</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Failed_</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="C22" t="n">

</xml_diff>